<commit_message>
Add fix and update demand projection for European countries
</commit_message>
<xml_diff>
--- a/raw_data_input/demand/Demand_TimeSeries_2030_NationalEstimates.xlsx
+++ b/raw_data_input/demand/Demand_TimeSeries_2030_NationalEstimates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\POMMES_public\pommes-data\raw_data_input\demand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CA5F31-46AD-4660-8234-FCF2407EFE71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE1484D-15C4-43FF-BFE2-F207DC597652}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15525" tabRatio="1000" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="38400" windowHeight="15525" tabRatio="1000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AT00" sheetId="2" r:id="rId1"/>
@@ -284,6 +284,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,7 +554,7 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -659,6 +662,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="33">
     <cellStyle name="Normal 2" xfId="27" xr:uid="{7889F082-7B8D-4B75-BD48-EDF49924D4CD}"/>
@@ -1964,7 +1968,7 @@
   <dimension ref="A1:AN11"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD8771"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,6 +2063,7 @@
       <c r="B5" s="16">
         <v>2030</v>
       </c>
+      <c r="C5" s="22"/>
       <c r="D5" s="42" t="s">
         <v>10</v>
       </c>
@@ -9993,7 +9998,7 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD8771"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12528,7 +12533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -16326,11 +16331,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD8771"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -16570,7 +16578,7 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="45">
         <v>81069</v>
       </c>
       <c r="D8" s="22">
@@ -16959,8 +16967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD8771"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>